<commit_message>
creation of development branch
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F370473F-8935-46B0-9A0F-1F4B714542A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102425F6-5A57-47B4-8DDE-4E01B6CC8777}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,30 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>fakewebstie.cum</t>
-  </si>
-  <si>
-    <t>col2</t>
-  </si>
-  <si>
-    <t>row2,colB</t>
-  </si>
-  <si>
-    <t>row3, col B</t>
-  </si>
-  <si>
-    <t>row4, col B</t>
   </si>
   <si>
     <t>https://google.com</t>
   </si>
   <si>
     <t>youtube.com</t>
+  </si>
+  <si>
+    <t>google.com/asdf</t>
+  </si>
+  <si>
+    <t>Response Code</t>
   </si>
 </sst>
 </file>
@@ -375,7 +366,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,31 +380,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>